<commit_message>
Customized Header with bold font, borders and background color
</commit_message>
<xml_diff>
--- a/Daily-Income-Expense-Sheets/2025-06-18-expenses.xlsx
+++ b/Daily-Income-Expense-Sheets/2025-06-18-expenses.xlsx
@@ -2,21 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,16 +25,24 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00808080"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,15 +50,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -414,39 +438,39 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Expense</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Balance</t>
         </is>
@@ -455,61 +479,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>16:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>selling paint</t>
+          <t>Purchasing a bicycle</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Purchase</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>300</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>200</v>
+        <v>-300</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>purchasing a tv</t>
+          <t>selling paint</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>purchase</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
       <c r="F3" t="n">
-        <v>-600</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>